<commit_message>
integration forms and auth
</commit_message>
<xml_diff>
--- a/forms_api/static/xlsx_files/filled_form/1/R.xlsx
+++ b/forms_api/static/xlsx_files/filled_form/1/R.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Counter</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Required</t>
+  </si>
+  <si>
+    <t>No value given</t>
   </si>
   <si>
     <t xml:space="preserve">button 1
@@ -54,17 +57,21 @@
 </t>
   </si>
   <si>
-    <t>No value given</t>
-  </si>
-  <si>
-    <t>string</t>
+    <t>First Title</t>
+  </si>
+  <si>
+    <t>Description 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.pexels.com/photos/268533/pexels-photo-268533.jpeg?cs=srgb&amp;dl=pexels-pixabay-268533.jpg&amp;fm=jpg
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +86,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -116,16 +130,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -467,20 +487,27 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>